<commit_message>
- warning: our license does not allow you to access a BIMcloud. dialog is now documented
</commit_message>
<xml_diff>
--- a/src/multiconn_archicad/dialog_handlers/win_int_handler_factory.xlsx
+++ b/src/multiconn_archicad/dialog_handlers/win_int_handler_factory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szamosi.mate\PycharmProjects\TSPC_TaskFlow\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szamosi.mate\PycharmProjects\MultiConnAC\src\multiconn_archicad\dialog_handlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A831E243-26D2-4657-9708-6EFDFD0AA574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565867B8-3DEC-4425-8286-D0C73FB02992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9955A94-9FDF-48E6-9CE7-3FE4E7B5F479}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E9955A94-9FDF-48E6-9CE7-3FE4E7B5F479}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="11">
+  <futureMetadata name="XLRICHVALUE" count="12">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -118,8 +118,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="11">
+  <valueMetadata count="12">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -153,12 +160,15 @@
     <bk>
       <rc t="1" v="10"/>
     </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
   <si>
     <t>Editing Conflict</t>
   </si>
@@ -603,6 +613,61 @@
   <si>
     <t xml:space="preserve">Do not handle
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opening a file in demo mode with libraris linked from bimcloud
+</t>
+  </si>
+  <si>
+    <t>Click "Continue"</t>
+  </si>
+  <si>
+    <t>{'succeeded': False, 'error': {'code': 4001, 'message': 'Invalid program status (there is an open modal dialog: Information)'}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dialog - 'TE_ST_01 - Archicad 27 DEMO'    (L-11, T-11, R3851, B2099)
+['TE_ST_01 - Archicad 27 DEMODialog', 'TE_ST_01 - Archicad 27 DEMO', 'Dialog', 'Dialog0', 'Dialog1']
+child_window(title="TE_ST_01 - Archicad 27 DEMO", control_type="Window")
+   | 
+   | Dialog - 'Information'    (L1503, T946, R2065, B1175)
+   | ['Information', 'InformationDialog', 'Dialog2']
+   | child_window(title="Information", control_type="Window")
+   |    | 
+   |    | Button - 'Continue'    (L1897, T1114, R2032, B1149)
+   |    | ['Button', 'ContinueButton', 'Continue', 'Button0', 'Button1']
+   |    | child_window(title="Continue", auto_id="1", control_type="Button")
+   |    | 
+   |    | Static - 'Your license does not allow you to access a BIMcloud.'    (L1597, T1006, R2032, B1056)
+   |    | ['Your license does not allow you to access a BIMcloud.', 'Static', 'Your license does not allow you to access a BIMcloud.Static', 'Your license does not allow you to access a BIMcloud.0', 'Your license does not allow you to access a BIMcloud.1', 'Static0', 'Static1']
+   |    | child_window(title="Your license does not allow you to access a BIMcloud.", auto_id="2", control_type="Text")
+   |    | 
+   |    | Image - 'Your license does not allow you to access a BIMcloud.'    (L1537, T1006, R1585, B1054)
+   |    | ['Your license does not allow you to access a BIMcloud.2', 'Your license does not allow you to access a BIMcloud.Image', 'Image']
+   |    | child_window(title="Your license does not allow you to access a BIMcloud.", auto_id="3", control_type="Image")
+   |    | 
+   |    | CheckBox - 'Do not display this dialog next time.'    (L1537, T1066, R2032, B1101)
+   |    | ['Do not display this dialog next time.CheckBox', 'CheckBox', 'Do not display this dialog next time.']
+   |    | child_window(title="Do not display this dialog next time.", auto_id="4", control_type="CheckBox")
+   |    | 
+   |    | TitleBar - ''    (L1538, T949, R2054, B991)
+   |    | ['Processing project dataTitleBar', 'TitleBar', 'TitleBar0', 'TitleBar1']
+   |    |    | 
+   |    |    | Menu - 'Rendszer'    (L1514, T957, R1547, B990)
+   |    |    | ['Rendszer', 'Menu', 'RendszerMenu', 'Rendszer0', 'Rendszer1', 'Menu0', 'Menu1', 'RendszerMenu0', 'RendszerMenu1']
+   |    |    | child_window(title="Rendszer", auto_id="MenuBar", control_type="MenuBar")
+   |    |    |    | 
+   |    |    |    | MenuItem - 'Rendszer'    (L1514, T957, R1547, B990)
+   |    |    |    | ['Rendszer2', 'RendszerMenuItem', 'MenuItem', 'RendszerMenuItem0', 'RendszerMenuItem1', 'MenuItem0', 'MenuItem1']
+   |    |    |    | child_window(title="Rendszer", control_type="MenuItem")
+   |    |    | 
+   |    |    | Button - 'Környezetfüggő súgó'    (L1913, T947, R1984, B991)
+   |    |    | ['Környezetfüggő súgó', 'Button2', 'Környezetfüggő súgóButton']
+   |    |    | child_window(title="Környezetfüggő súgó", control_type="Button")
+   |    |    | 
+   |    |    | Button - 'Bezárás'    (L1984, T947, R2055, B991)
+   |    |    | ['Button3', 'BezárásButton', 'Bezárás', 'BezárásButton0', 'BezárásButton1', 'Bezárás0', 'Bezárás1']
+   |    |    | child_window(title="Bezárás", control_type="Button")</t>
   </si>
 </sst>
 </file>
@@ -769,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -837,9 +902,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -848,9 +910,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -866,23 +925,6 @@
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -968,6 +1010,23 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1207,7 +1266,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="11">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="12">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -1252,6 +1311,10 @@
     <v>10</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -1277,6 +1340,7 @@
   <rel r:id="rId9"/>
   <rel r:id="rId10"/>
   <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
 </richValueRels>
 </file>
 
@@ -1291,12 +1355,12 @@
     <tableColumn id="2" xr3:uid="{6954D1A2-53A8-4900-AA33-7216B5084FCC}" name="When does it happen?" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{6D83DCD0-0B03-4F72-8576-A270E426082E}" name="Name of dialog" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{F3C1F246-E460-4DF4-AE7A-4175B5A8974D}" name="Printscreen" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{120DA47D-E344-4E03-9E04-076163F7AA11}" name="What do we do about it?" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{B3CFCE95-FDE3-4875-AD95-139718F6FB15}" name="Is alive Returns" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{58834A24-0A9E-4AC6-B150-34FDB1E340A4}" name="Is the message Unique?" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{59492D85-815E-40A9-934D-A53C6A553F3C}" name="Enter" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{E16387AF-76F9-4961-8D37-CC3D46A075FE}" name="ESC" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{B73E5C89-6664-4683-88ED-9B14E39B599A}" name="Pywinauto" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{120DA47D-E344-4E03-9E04-076163F7AA11}" name="What do we do about it?" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{B3CFCE95-FDE3-4875-AD95-139718F6FB15}" name="Is alive Returns" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{58834A24-0A9E-4AC6-B150-34FDB1E340A4}" name="Is the message Unique?" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{59492D85-815E-40A9-934D-A53C6A553F3C}" name="Enter" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{E16387AF-76F9-4961-8D37-CC3D46A075FE}" name="ESC" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{B73E5C89-6664-4683-88ED-9B14E39B599A}" name="Pywinauto" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1621,27 +1685,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5F192C-49AA-4D18-8AB1-6BB07877A33B}">
   <dimension ref="A1:DY40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="67.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="67.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" customWidth="1"/>
-    <col min="10" max="10" width="61.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7109375" style="1"/>
+    <col min="10" max="10" width="61.81640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="25.453125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:129" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:129" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>42</v>
       </c>
@@ -1675,7 +1739,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>60</v>
       </c>
@@ -1709,7 +1773,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>60</v>
       </c>
@@ -1743,7 +1807,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>60</v>
       </c>
@@ -1777,7 +1841,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>60</v>
       </c>
@@ -1811,7 +1875,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>60</v>
       </c>
@@ -1841,7 +1905,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>60</v>
       </c>
@@ -1875,7 +1939,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>60</v>
       </c>
@@ -1909,41 +1973,41 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="25" t="e" vm="6">
+      <c r="D9" s="24" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="28" t="s">
         <v>39</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>60</v>
       </c>
@@ -1977,8 +2041,8 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2009,8 +2073,8 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+    <row r="12" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2033,8 +2097,8 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:129" s="4" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+    <row r="13" spans="1:129" s="4" customFormat="1" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -2045,7 +2109,7 @@
       <c r="E13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="26" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="20" t="s">
@@ -2057,129 +2121,129 @@
       <c r="I13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="23"/>
-      <c r="AF13" s="23"/>
-      <c r="AG13" s="23"/>
-      <c r="AH13" s="23"/>
-      <c r="AI13" s="23"/>
-      <c r="AJ13" s="23"/>
-      <c r="AK13" s="23"/>
-      <c r="AL13" s="23"/>
-      <c r="AM13" s="23"/>
-      <c r="AN13" s="23"/>
-      <c r="AO13" s="23"/>
-      <c r="AP13" s="23"/>
-      <c r="AQ13" s="23"/>
-      <c r="AR13" s="23"/>
-      <c r="AS13" s="23"/>
-      <c r="AT13" s="23"/>
-      <c r="AU13" s="23"/>
-      <c r="AV13" s="23"/>
-      <c r="AW13" s="23"/>
-      <c r="AX13" s="23"/>
-      <c r="AY13" s="23"/>
-      <c r="AZ13" s="23"/>
-      <c r="BA13" s="23"/>
-      <c r="BB13" s="23"/>
-      <c r="BC13" s="23"/>
-      <c r="BD13" s="23"/>
-      <c r="BE13" s="23"/>
-      <c r="BF13" s="23"/>
-      <c r="BG13" s="23"/>
-      <c r="BH13" s="23"/>
-      <c r="BI13" s="23"/>
-      <c r="BJ13" s="23"/>
-      <c r="BK13" s="23"/>
-      <c r="BL13" s="23"/>
-      <c r="BM13" s="23"/>
-      <c r="BN13" s="23"/>
-      <c r="BO13" s="23"/>
-      <c r="BP13" s="23"/>
-      <c r="BQ13" s="23"/>
-      <c r="BR13" s="23"/>
-      <c r="BS13" s="23"/>
-      <c r="BT13" s="23"/>
-      <c r="BU13" s="23"/>
-      <c r="BV13" s="23"/>
-      <c r="BW13" s="23"/>
-      <c r="BX13" s="23"/>
-      <c r="BY13" s="23"/>
-      <c r="BZ13" s="23"/>
-      <c r="CA13" s="23"/>
-      <c r="CB13" s="23"/>
-      <c r="CC13" s="23"/>
-      <c r="CD13" s="23"/>
-      <c r="CE13" s="23"/>
-      <c r="CF13" s="23"/>
-      <c r="CG13" s="23"/>
-      <c r="CH13" s="23"/>
-      <c r="CI13" s="23"/>
-      <c r="CJ13" s="23"/>
-      <c r="CK13" s="23"/>
-      <c r="CL13" s="23"/>
-      <c r="CM13" s="23"/>
-      <c r="CN13" s="23"/>
-      <c r="CO13" s="23"/>
-      <c r="CP13" s="23"/>
-      <c r="CQ13" s="23"/>
-      <c r="CR13" s="23"/>
-      <c r="CS13" s="23"/>
-      <c r="CT13" s="23"/>
-      <c r="CU13" s="23"/>
-      <c r="CV13" s="23"/>
-      <c r="CW13" s="23"/>
-      <c r="CX13" s="23"/>
-      <c r="CY13" s="23"/>
-      <c r="CZ13" s="23"/>
-      <c r="DA13" s="23"/>
-      <c r="DB13" s="23"/>
-      <c r="DC13" s="23"/>
-      <c r="DD13" s="23"/>
-      <c r="DE13" s="23"/>
-      <c r="DF13" s="23"/>
-      <c r="DG13" s="23"/>
-      <c r="DH13" s="23"/>
-      <c r="DI13" s="23"/>
-      <c r="DJ13" s="23"/>
-      <c r="DK13" s="23"/>
-      <c r="DL13" s="23"/>
-      <c r="DM13" s="23"/>
-      <c r="DN13" s="23"/>
-      <c r="DO13" s="23"/>
-      <c r="DP13" s="23"/>
-      <c r="DQ13" s="23"/>
-      <c r="DR13" s="23"/>
-      <c r="DS13" s="23"/>
-      <c r="DT13" s="23"/>
-      <c r="DU13" s="23"/>
-      <c r="DV13" s="23"/>
-      <c r="DW13" s="23"/>
-      <c r="DX13" s="23"/>
-      <c r="DY13" s="23"/>
-    </row>
-    <row r="14" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="J13" s="27"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="1"/>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="1"/>
+      <c r="BE13" s="1"/>
+      <c r="BF13" s="1"/>
+      <c r="BG13" s="1"/>
+      <c r="BH13" s="1"/>
+      <c r="BI13" s="1"/>
+      <c r="BJ13" s="1"/>
+      <c r="BK13" s="1"/>
+      <c r="BL13" s="1"/>
+      <c r="BM13" s="1"/>
+      <c r="BN13" s="1"/>
+      <c r="BO13" s="1"/>
+      <c r="BP13" s="1"/>
+      <c r="BQ13" s="1"/>
+      <c r="BR13" s="1"/>
+      <c r="BS13" s="1"/>
+      <c r="BT13" s="1"/>
+      <c r="BU13" s="1"/>
+      <c r="BV13" s="1"/>
+      <c r="BW13" s="1"/>
+      <c r="BX13" s="1"/>
+      <c r="BY13" s="1"/>
+      <c r="BZ13" s="1"/>
+      <c r="CA13" s="1"/>
+      <c r="CB13" s="1"/>
+      <c r="CC13" s="1"/>
+      <c r="CD13" s="1"/>
+      <c r="CE13" s="1"/>
+      <c r="CF13" s="1"/>
+      <c r="CG13" s="1"/>
+      <c r="CH13" s="1"/>
+      <c r="CI13" s="1"/>
+      <c r="CJ13" s="1"/>
+      <c r="CK13" s="1"/>
+      <c r="CL13" s="1"/>
+      <c r="CM13" s="1"/>
+      <c r="CN13" s="1"/>
+      <c r="CO13" s="1"/>
+      <c r="CP13" s="1"/>
+      <c r="CQ13" s="1"/>
+      <c r="CR13" s="1"/>
+      <c r="CS13" s="1"/>
+      <c r="CT13" s="1"/>
+      <c r="CU13" s="1"/>
+      <c r="CV13" s="1"/>
+      <c r="CW13" s="1"/>
+      <c r="CX13" s="1"/>
+      <c r="CY13" s="1"/>
+      <c r="CZ13" s="1"/>
+      <c r="DA13" s="1"/>
+      <c r="DB13" s="1"/>
+      <c r="DC13" s="1"/>
+      <c r="DD13" s="1"/>
+      <c r="DE13" s="1"/>
+      <c r="DF13" s="1"/>
+      <c r="DG13" s="1"/>
+      <c r="DH13" s="1"/>
+      <c r="DI13" s="1"/>
+      <c r="DJ13" s="1"/>
+      <c r="DK13" s="1"/>
+      <c r="DL13" s="1"/>
+      <c r="DM13" s="1"/>
+      <c r="DN13" s="1"/>
+      <c r="DO13" s="1"/>
+      <c r="DP13" s="1"/>
+      <c r="DQ13" s="1"/>
+      <c r="DR13" s="1"/>
+      <c r="DS13" s="1"/>
+      <c r="DT13" s="1"/>
+      <c r="DU13" s="1"/>
+      <c r="DV13" s="1"/>
+      <c r="DW13" s="1"/>
+      <c r="DX13" s="1"/>
+      <c r="DY13" s="1"/>
+    </row>
+    <row r="14" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="20"/>
@@ -2192,7 +2256,7 @@
       <c r="E14" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="26" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -2210,8 +2274,8 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -2244,21 +2308,39 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:129" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="9"/>
+      <c r="B16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2272,7 +2354,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2286,7 +2368,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2300,7 +2382,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2314,7 +2396,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2328,7 +2410,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2342,7 +2424,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2356,7 +2438,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2370,7 +2452,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2384,7 +2466,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2398,7 +2480,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2412,7 +2494,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2426,7 +2508,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2440,7 +2522,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2454,7 +2536,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2468,7 +2550,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2482,14 +2564,14 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="200.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor project handlers and add timeout parameter
Introduced `ProjectOpenParams` data class to simplify parameter management in project handlers. Added a timeout parameter to `post_command` and `post_tapir_command` calls for better control. Simplified and structured the project opening workflow with clearer inputs and optional demo flag support.
</commit_message>
<xml_diff>
--- a/src/multiconn_archicad/dialog_handlers/win_int_handler_factory.xlsx
+++ b/src/multiconn_archicad/dialog_handlers/win_int_handler_factory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szamosi.mate\PycharmProjects\MultiConnAC\src\multiconn_archicad\dialog_handlers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szami\Documents\python\multiconn_archicad\src\multiconn_archicad\dialog_handlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565867B8-3DEC-4425-8286-D0C73FB02992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1BE4F2-B10F-40AE-9B2E-E20C929C313E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E9955A94-9FDF-48E6-9CE7-3FE4E7B5F479}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9955A94-9FDF-48E6-9CE7-3FE4E7B5F479}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -674,7 +672,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1226,7 +1224,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1685,27 +1683,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5F192C-49AA-4D18-8AB1-6BB07877A33B}">
   <dimension ref="A1:DY40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="67.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="67.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" customWidth="1"/>
-    <col min="10" max="10" width="61.81640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="25.453125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="1"/>
+    <col min="10" max="10" width="61.875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="25.5" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:129" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:129">
       <c r="A1" s="16" t="s">
         <v>42</v>
       </c>
@@ -1739,7 +1737,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:129" ht="200.1" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>60</v>
       </c>
@@ -1773,7 +1771,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:129" ht="200.1" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>60</v>
       </c>
@@ -1807,7 +1805,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:129" ht="200.1" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>60</v>
       </c>
@@ -1841,7 +1839,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:129" ht="200.1" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>60</v>
       </c>
@@ -1875,7 +1873,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:129" ht="200.1" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>60</v>
       </c>
@@ -1905,7 +1903,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:129" ht="200.1" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>60</v>
       </c>
@@ -1939,7 +1937,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:129" ht="200.1" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>60</v>
       </c>
@@ -1973,7 +1971,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:129" ht="200.1" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -2007,7 +2005,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:129" ht="200.1" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>60</v>
       </c>
@@ -2041,7 +2039,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:129" ht="200.1" customHeight="1">
       <c r="A11" s="23" t="s">
         <v>61</v>
       </c>
@@ -2073,7 +2071,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:129" ht="200.1" customHeight="1">
       <c r="A12" s="23" t="s">
         <v>61</v>
       </c>
@@ -2097,7 +2095,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:129" s="4" customFormat="1" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:129" s="4" customFormat="1" ht="200.1" customHeight="1">
       <c r="A13" s="23" t="s">
         <v>61</v>
       </c>
@@ -2242,7 +2240,7 @@
       <c r="DX13" s="1"/>
       <c r="DY13" s="1"/>
     </row>
-    <row r="14" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:129" ht="200.1" customHeight="1">
       <c r="A14" s="23" t="s">
         <v>61</v>
       </c>
@@ -2274,7 +2272,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:129" ht="200.1" customHeight="1">
       <c r="A15" s="23" t="s">
         <v>61</v>
       </c>
@@ -2308,7 +2306,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:129" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:129" ht="200.1" customHeight="1">
       <c r="A16" s="13"/>
       <c r="B16" s="10" t="s">
         <v>62</v>
@@ -2340,7 +2338,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="200.1" customHeight="1">
       <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2354,7 +2352,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="200.1" customHeight="1">
       <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2368,7 +2366,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="200.1" customHeight="1">
       <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2382,7 +2380,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="200.1" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2396,7 +2394,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="200.1" customHeight="1">
       <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2410,7 +2408,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="200.1" customHeight="1">
       <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2424,7 +2422,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="200.1" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2438,7 +2436,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="200.1" customHeight="1">
       <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2452,7 +2450,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="200.1" customHeight="1">
       <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2466,7 +2464,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="200.1" customHeight="1">
       <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2480,7 +2478,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="200.1" customHeight="1">
       <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2494,7 +2492,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="200.1" customHeight="1">
       <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2508,7 +2506,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="200.1" customHeight="1">
       <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2522,7 +2520,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="200.1" customHeight="1">
       <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2536,7 +2534,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="200.1" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2550,7 +2548,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="200.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="200.1" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2564,14 +2562,14 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="200.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="200.1" customHeight="1"/>
+    <row r="34" ht="200.1" customHeight="1"/>
+    <row r="35" ht="200.1" customHeight="1"/>
+    <row r="36" ht="200.1" customHeight="1"/>
+    <row r="37" ht="200.1" customHeight="1"/>
+    <row r="38" ht="200.1" customHeight="1"/>
+    <row r="39" ht="200.1" customHeight="1"/>
+    <row r="40" ht="200.1" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>